<commit_message>
add bent acrylic shield
</commit_message>
<xml_diff>
--- a/laserresin5.xlsx
+++ b/laserresin5.xlsx
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +1886,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>10</v>
+        <v>12.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>